<commit_message>
Updated test cases with proper data
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Master_Sheet.xlsx
+++ b/src/test/resources/testData/Master_Sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TestingFramework\FrameWork\src\test\resources\testData\"/>
     </mc:Choice>
@@ -19,10 +19,11 @@
     <sheet name="Login" sheetId="3" r:id="rId4"/>
     <sheet name="Raw_Data" sheetId="5" r:id="rId5"/>
     <sheet name="dk_data" sheetId="6" r:id="rId6"/>
+    <sheet name="NewSheet" r:id="rId10" sheetId="8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="118">
   <si>
     <t xml:space="preserve">Sr. No </t>
   </si>
@@ -399,7 +400,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,7 +432,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,6 +443,16 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
       </patternFill>
     </fill>
   </fills>
@@ -472,7 +484,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -491,6 +503,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -780,9 +793,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.26953125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.54296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -938,10 +951,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.36328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1031,8 +1044,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{0A278EC2-A868-4640-9B9B-E337473E1DE4}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{EC82C501-277D-4713-ADA7-62B53985B7DE}"/>
+    <hyperlink ref="C3" r:id="rId6" xr:uid="{0A278EC2-A868-4640-9B9B-E337473E1DE4}"/>
+    <hyperlink ref="C7" r:id="rId7" xr:uid="{EC82C501-277D-4713-ADA7-62B53985B7DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1047,13 +1060,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="28.36328125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.6328125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1561,17 +1574,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D25" r:id="rId1" xr:uid="{12C3EA19-F519-4A98-ADB3-157E1950AA12}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{E14532F3-C412-4887-A037-8192E3D179FF}"/>
-    <hyperlink ref="D9" r:id="rId3" xr:uid="{071A4136-D819-4359-A3F5-9E1C626878C9}"/>
-    <hyperlink ref="D13" r:id="rId4" xr:uid="{BCE147EC-CE76-4960-B078-A3C4DC09AB74}"/>
-    <hyperlink ref="D17" r:id="rId5" xr:uid="{79532CE8-01F2-4DDD-8E3F-B776F679A270}"/>
-    <hyperlink ref="D21" r:id="rId6" xr:uid="{D5A0F6CC-ACE3-4515-BA5B-3331943C440E}"/>
-    <hyperlink ref="D29" r:id="rId7" xr:uid="{D866BF4E-0F9A-4DA8-833C-6B1BC5058076}"/>
-    <hyperlink ref="D4" r:id="rId8" xr:uid="{432F92E9-A5A6-43EF-AC91-340D465B25CB}"/>
-    <hyperlink ref="D5" r:id="rId9" xr:uid="{F0074779-A850-4FDA-A3A9-C8661EF2177E}"/>
-    <hyperlink ref="D30" r:id="rId10" xr:uid="{796235E4-DDA6-4C9C-8896-836995CD48CB}"/>
-    <hyperlink ref="D31" r:id="rId11" xr:uid="{07E9D520-BBD5-4118-A94F-4FE2191D0738}"/>
+    <hyperlink ref="D25" r:id="rId24" xr:uid="{12C3EA19-F519-4A98-ADB3-157E1950AA12}"/>
+    <hyperlink ref="D3" r:id="rId25" xr:uid="{E14532F3-C412-4887-A037-8192E3D179FF}"/>
+    <hyperlink ref="D9" r:id="rId26" xr:uid="{071A4136-D819-4359-A3F5-9E1C626878C9}"/>
+    <hyperlink ref="D13" r:id="rId27" xr:uid="{BCE147EC-CE76-4960-B078-A3C4DC09AB74}"/>
+    <hyperlink ref="D17" r:id="rId28" xr:uid="{79532CE8-01F2-4DDD-8E3F-B776F679A270}"/>
+    <hyperlink ref="D21" r:id="rId29" xr:uid="{D5A0F6CC-ACE3-4515-BA5B-3331943C440E}"/>
+    <hyperlink ref="D29" r:id="rId30" xr:uid="{D866BF4E-0F9A-4DA8-833C-6B1BC5058076}"/>
+    <hyperlink ref="D4" r:id="rId31" xr:uid="{432F92E9-A5A6-43EF-AC91-340D465B25CB}"/>
+    <hyperlink ref="D5" r:id="rId32" xr:uid="{F0074779-A850-4FDA-A3A9-C8661EF2177E}"/>
+    <hyperlink ref="D30" r:id="rId33" xr:uid="{796235E4-DDA6-4C9C-8896-836995CD48CB}"/>
+    <hyperlink ref="D31" r:id="rId34" xr:uid="{07E9D520-BBD5-4118-A94F-4FE2191D0738}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
@@ -1588,7 +1601,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="18.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1714,8 +1727,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Test@123" xr:uid="{62FB09AA-FF9A-4396-8638-30673F43805C}"/>
-    <hyperlink ref="B3:B11" r:id="rId2" display="Test@123" xr:uid="{0E4BF116-5CAD-4922-A306-D0A853A20CF3}"/>
+    <hyperlink ref="B2" r:id="rId5" display="Test@123" xr:uid="{62FB09AA-FF9A-4396-8638-30673F43805C}"/>
+    <hyperlink ref="B3:B11" r:id="rId6" display="Test@123" xr:uid="{0E4BF116-5CAD-4922-A306-D0A853A20CF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1809,9 +1822,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Test@123" xr:uid="{76343734-6838-4D0F-BE13-8F01945823D7}"/>
-    <hyperlink ref="C3" r:id="rId2" display="Test@123" xr:uid="{44A3BC44-C40B-47EE-BEA9-119C6AA67486}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{2C9C570E-4BEC-4DBD-9675-27102FAED252}"/>
+    <hyperlink ref="C2" r:id="rId7" display="Test@123" xr:uid="{76343734-6838-4D0F-BE13-8F01945823D7}"/>
+    <hyperlink ref="C3" r:id="rId8" display="Test@123" xr:uid="{44A3BC44-C40B-47EE-BEA9-119C6AA67486}"/>
+    <hyperlink ref="B3" r:id="rId9" xr:uid="{2C9C570E-4BEC-4DBD-9675-27102FAED252}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1827,10 +1840,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7265625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.26953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.1796875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1877,9 +1890,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{61D6891D-24CB-4568-814D-92C676634595}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{373F8C44-FF72-42CE-B5FD-FF6AEAF5A004}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{61D6891D-24CB-4568-814D-92C676634595}"/>
+    <hyperlink ref="B3" r:id="rId6" xr:uid="{373F8C44-FF72-42CE-B5FD-FF6AEAF5A004}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="14">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new test case social medialinktest
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Master_Sheet.xlsx
+++ b/src/test/resources/testData/Master_Sheet.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TestingFramework\FrameWork\src\test\resources\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51230403-8B5C-4A59-BD6A-3063ED3CC639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0E1A76D2-55D7-4E73-91AB-718EBE321A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,8 @@
     <sheet name="dk_data" sheetId="6" r:id="rId6"/>
     <sheet name="NewSheet" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:L16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="123">
   <si>
     <t xml:space="preserve">Sr. No </t>
   </si>
@@ -406,6 +402,9 @@
   </si>
   <si>
     <t>VerifyTitleOfByAutomation</t>
+  </si>
+  <si>
+    <t>VerifySocialMediaLinkTest</t>
   </si>
 </sst>
 </file>
@@ -791,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -862,10 +861,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -949,7 +948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4668CBAB-C452-40CE-A283-6DB616929218}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>